<commit_message>
Atualizando a tabela de treino
</commit_message>
<xml_diff>
--- a/dados_treino_bruto.xlsx
+++ b/dados_treino_bruto.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26920"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alinsperedu-my.sharepoint.com/personal/marialssac_al_insper_edu_br/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malus\CeDados\Naive_Bayes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E6B9554-012D-4853-81C6-BCCD7D1E81FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B3723AE-64EA-4236-9B0A-FC93C8212343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="10455" windowHeight="10905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="308">
   <si>
     <t>Mensagem</t>
   </si>
@@ -960,43 +960,19 @@
   </si>
   <si>
     <t>Entrega e Discordou</t>
-  </si>
-  <si>
-    <t>outros</t>
-  </si>
-  <si>
-    <t>Condição do livro e da compra</t>
-  </si>
-  <si>
-    <t>Intersecação</t>
-  </si>
-  <si>
-    <t>Livro Fraco</t>
-  </si>
-  <si>
-    <t>Intersecção</t>
-  </si>
-  <si>
-    <t>Discordou do livro</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1027,6 +1003,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -1111,13 +1094,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1127,32 +1110,49 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -1177,6 +1177,17 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1C49BE00-774E-4EF1-8F18-E2533087DEC0}" name="Tabela1" displayName="Tabela1" ref="A1:B301" totalsRowShown="0">
+  <autoFilter ref="A1:B301" xr:uid="{1C49BE00-774E-4EF1-8F18-E2533087DEC0}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{6BCBA133-5039-498D-BC5B-AEDB648FB4F1}" name="Mensagem" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{5191783E-2EE2-4021-A325-8406A392E240}" name="Target" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1464,26 +1475,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K308"/>
+  <dimension ref="A1:O310"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B238" zoomScale="70" zoomScaleNormal="10" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:K13"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="10" workbookViewId="0">
+      <selection activeCell="O310" sqref="O310"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
     <col min="2" max="2" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>2</v>
       </c>
@@ -1491,7 +1503,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>4</v>
       </c>
@@ -1505,7 +1517,7 @@
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>5</v>
       </c>
@@ -1519,7 +1531,7 @@
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>6</v>
       </c>
@@ -1533,7 +1545,7 @@
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>7</v>
       </c>
@@ -1547,7 +1559,7 @@
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>8</v>
       </c>
@@ -1561,7 +1573,7 @@
       <c r="J7" s="10"/>
       <c r="K7" s="10"/>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>9</v>
       </c>
@@ -1575,7 +1587,7 @@
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>10</v>
       </c>
@@ -1589,7 +1601,7 @@
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>11</v>
       </c>
@@ -1603,7 +1615,7 @@
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>12</v>
       </c>
@@ -1617,7 +1629,7 @@
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>13</v>
       </c>
@@ -1631,7 +1643,7 @@
       <c r="J12" s="10"/>
       <c r="K12" s="10"/>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>14</v>
       </c>
@@ -1645,7 +1657,7 @@
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>15</v>
       </c>
@@ -1653,7 +1665,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>16</v>
       </c>
@@ -1662,7 +1674,7 @@
       </c>
       <c r="H15" s="10"/>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>17</v>
       </c>
@@ -1670,7 +1682,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>18</v>
       </c>
@@ -1678,7 +1690,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>19</v>
       </c>
@@ -1686,7 +1698,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>21</v>
       </c>
@@ -1694,7 +1706,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>22</v>
       </c>
@@ -1702,7 +1714,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>23</v>
       </c>
@@ -1710,7 +1722,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>24</v>
       </c>
@@ -1718,7 +1730,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>25</v>
       </c>
@@ -1726,7 +1738,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>26</v>
       </c>
@@ -1734,7 +1746,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>27</v>
       </c>
@@ -1742,7 +1754,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>28</v>
       </c>
@@ -1750,7 +1762,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>29</v>
       </c>
@@ -1758,7 +1770,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>30</v>
       </c>
@@ -1766,7 +1778,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
         <v>31</v>
       </c>
@@ -1774,7 +1786,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>32</v>
       </c>
@@ -1782,7 +1794,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
         <v>33</v>
       </c>
@@ -1790,7 +1802,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
         <v>34</v>
       </c>
@@ -1798,7 +1810,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>35</v>
       </c>
@@ -1806,7 +1818,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>36</v>
       </c>
@@ -1814,7 +1826,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
         <v>37</v>
       </c>
@@ -1822,7 +1834,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
         <v>38</v>
       </c>
@@ -1830,7 +1842,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
         <v>39</v>
       </c>
@@ -1838,7 +1850,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>40</v>
       </c>
@@ -1846,7 +1858,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
         <v>41</v>
       </c>
@@ -1854,7 +1866,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
         <v>42</v>
       </c>
@@ -1862,7 +1874,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
         <v>43</v>
       </c>
@@ -1870,7 +1882,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:2" s="8" customFormat="1">
+    <row r="42" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
         <v>44</v>
       </c>
@@ -1878,7 +1890,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
         <v>45</v>
       </c>
@@ -1886,7 +1898,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
         <v>46</v>
       </c>
@@ -1894,7 +1906,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>47</v>
       </c>
@@ -1902,7 +1914,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
         <v>48</v>
       </c>
@@ -1910,1136 +1922,1136 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B47" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2">
+      <c r="B47" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B48" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" s="9" customFormat="1">
+      <c r="B48" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B49" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2">
+      <c r="B49" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B50" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2">
+      <c r="B50" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B51" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2">
+      <c r="B51" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B52" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
+      <c r="B52" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B53" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2">
+      <c r="B53" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B54" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2">
+      <c r="B54" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B55" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2">
+      <c r="B55" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B56" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2">
+      <c r="B56" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B57" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2">
+      <c r="B57" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B58" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2">
+      <c r="B58" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B59" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2">
+      <c r="B59" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B60" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2">
+      <c r="B60" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B61" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2">
+      <c r="B61" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B62" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2">
+      <c r="B62" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B63" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2">
+      <c r="B63" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B64" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2">
+      <c r="B64" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B65" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2">
+      <c r="B65" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B66" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2">
+      <c r="B66" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B67" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2">
+      <c r="B67" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B68" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2">
+      <c r="B68" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B69" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2">
+      <c r="B69" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B70" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2">
+      <c r="B70" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B71" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2">
+      <c r="B71" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B72" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2">
+      <c r="B72" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B73" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2">
+      <c r="B73" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B74" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2">
+      <c r="B74" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B75" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2">
+      <c r="B75" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B76" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2">
+      <c r="B76" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B77" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2">
+      <c r="B77" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B78" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2">
+      <c r="B78" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B79" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2">
+      <c r="B79" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B80" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2">
+      <c r="B80" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B81" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2">
+      <c r="B81" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B82" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2">
+      <c r="B82" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B83" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2">
+      <c r="B83" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B84" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2">
+      <c r="B84" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B85" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2">
+      <c r="B85" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B86" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2">
+      <c r="B86" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B87" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2">
+      <c r="B87" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B88" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2">
+      <c r="B88" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B89" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2">
+      <c r="B89" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B90" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2">
+      <c r="B90" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B91" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2">
+      <c r="B91" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B92" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2">
+      <c r="B92" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B93" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2">
+      <c r="B93" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B94" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2">
+      <c r="B94" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B95" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2">
+      <c r="B95" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B96" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2">
+      <c r="B96" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B97" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2">
+      <c r="B97" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B98" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2">
+      <c r="B98" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B99" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2">
+      <c r="B99" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B100" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2">
+      <c r="B100" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B101" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2">
+      <c r="B101" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B102" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2">
+      <c r="B102" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B103" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2">
+      <c r="B103" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B104" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2">
+      <c r="B104" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B105" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2">
+      <c r="B105" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B106" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2">
+      <c r="B106" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B107" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2">
+      <c r="B107" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B108" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2">
+      <c r="B108" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B109" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2">
+      <c r="B109" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B110" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2">
+      <c r="B110" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B111" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2">
+      <c r="B111" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B112" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2">
+      <c r="B112" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B113" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2">
+      <c r="B113" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="B114" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2">
+      <c r="B114" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B115" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2">
+      <c r="B115" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B116" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2">
+      <c r="B116" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B117" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2">
+      <c r="B117" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B118" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2">
+      <c r="B118" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="B119" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2">
+      <c r="B119" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B120" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2">
+      <c r="B120" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B121" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2">
+      <c r="B121" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="B122" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2">
+      <c r="B122" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B123" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2">
+      <c r="B123" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="B124" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2">
+      <c r="B124" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B125" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2">
+      <c r="B125" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B126" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2">
+      <c r="B126" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B127" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2">
+      <c r="B127" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="B128" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2">
+      <c r="B128" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B129" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2">
+      <c r="B129" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="B130" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2">
+      <c r="B130" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B131" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2">
+      <c r="B131" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="B132" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2">
+      <c r="B132" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="B133" s="17" t="s">
+      <c r="B133" s="16" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="134" spans="1:2">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="B134" s="17" t="s">
+      <c r="B134" s="16" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="135" spans="1:2">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="B135" s="17" t="s">
+      <c r="B135" s="16" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="136" spans="1:2">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="B136" s="17" t="s">
+      <c r="B136" s="16" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="137" spans="1:2">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="B137" s="17" t="s">
+      <c r="B137" s="16" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="138" spans="1:2">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="B138" s="17" t="s">
+      <c r="B138" s="16" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="139" spans="1:2">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="B139" s="17" t="s">
+      <c r="B139" s="16" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="140" spans="1:2">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B140" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2">
+      <c r="B140" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="B141" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2">
+      <c r="B141" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B142" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2">
+      <c r="B142" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="B143" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2">
+      <c r="B143" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B144" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2">
+      <c r="B144" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="B145" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2">
+      <c r="B145" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B146" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2">
+      <c r="B146" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B147" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2">
+      <c r="B147" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="B148" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2">
+      <c r="B148" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="B149" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2">
+      <c r="B149" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B150" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2">
+      <c r="B150" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B151" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2">
+      <c r="B151" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B152" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2">
+      <c r="B152" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B153" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2">
+      <c r="B153" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="B154" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2">
+      <c r="B154" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="B155" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2">
+      <c r="B155" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="B156" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2">
+      <c r="B156" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B157" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2">
+      <c r="B157" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B158" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2">
+      <c r="B158" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B159" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2">
+      <c r="B159" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B160" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="161" spans="1:8">
+      <c r="B160" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B161" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="162" spans="1:8">
+      <c r="B161" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="B162" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="163" spans="1:8">
+      <c r="B162" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B163" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="164" spans="1:8">
+      <c r="B163" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="B164" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="165" spans="1:8">
+      <c r="B164" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="B165" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="166" spans="1:8">
+      <c r="B165" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="B166" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="167" spans="1:8">
+      <c r="B166" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="B167" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="168" spans="1:8">
+      <c r="B167" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B168" s="18" t="s">
+      <c r="B168" s="17" t="s">
         <v>145</v>
       </c>
       <c r="H168" s="10"/>
     </row>
-    <row r="169" spans="1:8">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="B169" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="170" spans="1:8">
+      <c r="B169" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="B170" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="171" spans="1:8">
+      <c r="B170" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="B171" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="172" spans="1:8">
+      <c r="B171" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="B172" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="173" spans="1:8">
+      <c r="B172" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B173" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="174" spans="1:8">
+      <c r="B173" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="B174" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="175" spans="1:8">
+      <c r="B174" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="B175" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="176" spans="1:8">
+      <c r="B175" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="B176" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2">
+      <c r="B176" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="B177" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2">
+      <c r="B177" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="B178" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2">
+      <c r="B178" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="B179" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2">
+      <c r="B179" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="B180" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2">
+      <c r="B180" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="B181" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2">
+      <c r="B181" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="B182" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="183" spans="1:2">
+      <c r="B182" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B183" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="184" spans="1:2">
+      <c r="B183" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="B184" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="185" spans="1:2">
+      <c r="B184" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="B185" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="186" spans="1:2">
+      <c r="B185" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="B186" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="187" spans="1:2">
+      <c r="B186" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="B187" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="188" spans="1:2">
+      <c r="B187" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>193</v>
       </c>
@@ -3047,7 +3059,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="189" spans="1:2">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>195</v>
       </c>
@@ -3055,7 +3067,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="190" spans="1:2">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>196</v>
       </c>
@@ -3063,7 +3075,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="191" spans="1:2">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>197</v>
       </c>
@@ -3071,7 +3083,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="192" spans="1:2">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>198</v>
       </c>
@@ -3079,7 +3091,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="193" spans="1:2">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>199</v>
       </c>
@@ -3087,7 +3099,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="194" spans="1:2">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>200</v>
       </c>
@@ -3095,7 +3107,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="195" spans="1:2">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
         <v>201</v>
       </c>
@@ -3103,7 +3115,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="196" spans="1:2">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>202</v>
       </c>
@@ -3111,7 +3123,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="197" spans="1:2">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
         <v>203</v>
       </c>
@@ -3119,7 +3131,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="198" spans="1:2" s="9" customFormat="1">
+    <row r="198" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>204</v>
       </c>
@@ -3127,7 +3139,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="199" spans="1:2">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
         <v>205</v>
       </c>
@@ -3135,7 +3147,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="200" spans="1:2">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
         <v>206</v>
       </c>
@@ -3143,7 +3155,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="201" spans="1:2">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
         <v>207</v>
       </c>
@@ -3151,7 +3163,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="202" spans="1:2">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
         <v>208</v>
       </c>
@@ -3159,7 +3171,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="203" spans="1:2">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" s="4" t="s">
         <v>209</v>
       </c>
@@ -3167,7 +3179,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="204" spans="1:2">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
         <v>210</v>
       </c>
@@ -3175,7 +3187,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="205" spans="1:2">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
         <v>211</v>
       </c>
@@ -3183,7 +3195,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="206" spans="1:2">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
         <v>212</v>
       </c>
@@ -3191,7 +3203,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="207" spans="1:2">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
         <v>213</v>
       </c>
@@ -3199,7 +3211,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="208" spans="1:2">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
         <v>214</v>
       </c>
@@ -3207,7 +3219,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="209" spans="1:2">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
         <v>215</v>
       </c>
@@ -3215,7 +3227,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="210" spans="1:2">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
         <v>216</v>
       </c>
@@ -3223,7 +3235,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="211" spans="1:2">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
         <v>217</v>
       </c>
@@ -3231,7 +3243,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="212" spans="1:2">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
         <v>218</v>
       </c>
@@ -3239,7 +3251,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="213" spans="1:2">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
         <v>219</v>
       </c>
@@ -3247,7 +3259,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="214" spans="1:2">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
         <v>220</v>
       </c>
@@ -3255,7 +3267,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="215" spans="1:2">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
         <v>221</v>
       </c>
@@ -3263,7 +3275,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="216" spans="1:2">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
         <v>222</v>
       </c>
@@ -3271,7 +3283,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="217" spans="1:2">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
         <v>223</v>
       </c>
@@ -3279,7 +3291,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="218" spans="1:2">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
         <v>224</v>
       </c>
@@ -3287,7 +3299,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="219" spans="1:2">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
         <v>225</v>
       </c>
@@ -3295,7 +3307,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="220" spans="1:2">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
         <v>226</v>
       </c>
@@ -3303,7 +3315,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="221" spans="1:2">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
         <v>227</v>
       </c>
@@ -3311,7 +3323,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="222" spans="1:2" s="9" customFormat="1">
+    <row r="222" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
         <v>228</v>
       </c>
@@ -3319,7 +3331,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="223" spans="1:2">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
         <v>229</v>
       </c>
@@ -3327,7 +3339,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="224" spans="1:2">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
         <v>230</v>
       </c>
@@ -3335,7 +3347,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="225" spans="1:2">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
         <v>231</v>
       </c>
@@ -3343,7 +3355,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="226" spans="1:2">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
         <v>232</v>
       </c>
@@ -3351,7 +3363,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="227" spans="1:2">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
         <v>233</v>
       </c>
@@ -3359,7 +3371,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="228" spans="1:2">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
         <v>234</v>
       </c>
@@ -3367,7 +3379,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="229" spans="1:2" s="9" customFormat="1">
+    <row r="229" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
         <v>235</v>
       </c>
@@ -3375,7 +3387,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="230" spans="1:2">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
         <v>236</v>
       </c>
@@ -3383,7 +3395,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="231" spans="1:2">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
         <v>237</v>
       </c>
@@ -3391,7 +3403,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="232" spans="1:2">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
         <v>238</v>
       </c>
@@ -3399,7 +3411,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="233" spans="1:2">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
         <v>239</v>
       </c>
@@ -3407,7 +3419,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="234" spans="1:2">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
         <v>240</v>
       </c>
@@ -3415,7 +3427,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="235" spans="1:2">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
         <v>241</v>
       </c>
@@ -3423,7 +3435,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="236" spans="1:2">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
         <v>242</v>
       </c>
@@ -3431,7 +3443,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="237" spans="1:2">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
         <v>243</v>
       </c>
@@ -3439,7 +3451,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="238" spans="1:2">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
         <v>244</v>
       </c>
@@ -3447,7 +3459,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="239" spans="1:2">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
         <v>245</v>
       </c>
@@ -3455,7 +3467,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="240" spans="1:2">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
         <v>246</v>
       </c>
@@ -3463,7 +3475,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="241" spans="1:2">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
         <v>209</v>
       </c>
@@ -3471,7 +3483,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="242" spans="1:2">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
         <v>247</v>
       </c>
@@ -3479,7 +3491,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="243" spans="1:2">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
         <v>248</v>
       </c>
@@ -3487,7 +3499,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="244" spans="1:2">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
         <v>249</v>
       </c>
@@ -3495,7 +3507,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="245" spans="1:2">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
         <v>250</v>
       </c>
@@ -3503,7 +3515,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="246" spans="1:2">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
         <v>251</v>
       </c>
@@ -3511,7 +3523,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="247" spans="1:2">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
         <v>252</v>
       </c>
@@ -3519,7 +3531,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="248" spans="1:2">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
         <v>253</v>
       </c>
@@ -3527,7 +3539,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="249" spans="1:2">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
         <v>254</v>
       </c>
@@ -3535,7 +3547,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="250" spans="1:2">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
         <v>255</v>
       </c>
@@ -3543,7 +3555,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="251" spans="1:2">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
         <v>256</v>
       </c>
@@ -3551,7 +3563,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="252" spans="1:2">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
         <v>257</v>
       </c>
@@ -3559,7 +3571,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="253" spans="1:2">
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
         <v>258</v>
       </c>
@@ -3567,7 +3579,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="254" spans="1:2">
+    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
         <v>259</v>
       </c>
@@ -3575,7 +3587,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="255" spans="1:2">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
         <v>260</v>
       </c>
@@ -3583,7 +3595,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="256" spans="1:2">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
         <v>261</v>
       </c>
@@ -3591,7 +3603,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="257" spans="1:2">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
         <v>262</v>
       </c>
@@ -3599,7 +3611,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="258" spans="1:2">
+    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
         <v>263</v>
       </c>
@@ -3607,7 +3619,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="259" spans="1:2">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
         <v>264</v>
       </c>
@@ -3615,7 +3627,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="260" spans="1:2">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
         <v>265</v>
       </c>
@@ -3623,7 +3635,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="261" spans="1:2">
+    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
         <v>266</v>
       </c>
@@ -3631,7 +3643,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="262" spans="1:2">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
         <v>267</v>
       </c>
@@ -3639,7 +3651,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="263" spans="1:2">
+    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
         <v>268</v>
       </c>
@@ -3647,7 +3659,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="264" spans="1:2">
+    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
         <v>216</v>
       </c>
@@ -3655,7 +3667,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="265" spans="1:2">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
         <v>269</v>
       </c>
@@ -3663,7 +3675,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="266" spans="1:2">
+    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
         <v>270</v>
       </c>
@@ -3671,7 +3683,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="267" spans="1:2">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
         <v>271</v>
       </c>
@@ -3679,7 +3691,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="268" spans="1:2">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
         <v>272</v>
       </c>
@@ -3687,7 +3699,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="269" spans="1:2">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
         <v>273</v>
       </c>
@@ -3695,7 +3707,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="270" spans="1:2">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
         <v>274</v>
       </c>
@@ -3703,7 +3715,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="271" spans="1:2">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
         <v>275</v>
       </c>
@@ -3711,7 +3723,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="272" spans="1:2">
+    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
         <v>276</v>
       </c>
@@ -3719,7 +3731,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="273" spans="1:2">
+    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273" s="1" t="s">
         <v>277</v>
       </c>
@@ -3727,7 +3739,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="274" spans="1:2">
+    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
         <v>278</v>
       </c>
@@ -3735,7 +3747,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="275" spans="1:2">
+    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A275" s="1" t="s">
         <v>279</v>
       </c>
@@ -3743,7 +3755,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="276" spans="1:2">
+    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276" s="1" t="s">
         <v>280</v>
       </c>
@@ -3751,7 +3763,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="277" spans="1:2">
+    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
         <v>281</v>
       </c>
@@ -3759,7 +3771,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="278" spans="1:2">
+    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
         <v>282</v>
       </c>
@@ -3767,7 +3779,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="279" spans="1:2">
+    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
         <v>283</v>
       </c>
@@ -3775,7 +3787,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="280" spans="1:2">
+    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
         <v>284</v>
       </c>
@@ -3783,7 +3795,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="281" spans="1:2">
+    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A281" s="1" t="s">
         <v>285</v>
       </c>
@@ -3791,7 +3803,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="282" spans="1:2">
+    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
         <v>286</v>
       </c>
@@ -3799,7 +3811,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="283" spans="1:2">
+    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A283" s="1" t="s">
         <v>287</v>
       </c>
@@ -3807,7 +3819,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="284" spans="1:2">
+    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A284" s="1" t="s">
         <v>288</v>
       </c>
@@ -3815,7 +3827,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="285" spans="1:2">
+    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A285" s="1" t="s">
         <v>289</v>
       </c>
@@ -3823,7 +3835,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="286" spans="1:2">
+    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
         <v>290</v>
       </c>
@@ -3831,7 +3843,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="287" spans="1:2">
+    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A287" s="1" t="s">
         <v>291</v>
       </c>
@@ -3839,7 +3851,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="288" spans="1:2">
+    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A288" s="1" t="s">
         <v>292</v>
       </c>
@@ -3847,7 +3859,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="289" spans="1:9">
+    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
         <v>293</v>
       </c>
@@ -3855,7 +3867,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="290" spans="1:9">
+    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
         <v>294</v>
       </c>
@@ -3863,7 +3875,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="291" spans="1:9">
+    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A291" s="1" t="s">
         <v>295</v>
       </c>
@@ -3871,7 +3883,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="292" spans="1:9">
+    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
         <v>296</v>
       </c>
@@ -3879,7 +3891,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="293" spans="1:9">
+    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
         <v>297</v>
       </c>
@@ -3887,7 +3899,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="294" spans="1:9">
+    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A294" s="1" t="s">
         <v>298</v>
       </c>
@@ -3895,7 +3907,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="295" spans="1:9">
+    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A295" s="1" t="s">
         <v>299</v>
       </c>
@@ -3903,7 +3915,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="296" spans="1:9">
+    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
         <v>300</v>
       </c>
@@ -3911,7 +3923,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="297" spans="1:9">
+    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A297" s="1" t="s">
         <v>301</v>
       </c>
@@ -3919,7 +3931,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="298" spans="1:9">
+    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
         <v>302</v>
       </c>
@@ -3927,7 +3939,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="299" spans="1:9">
+    <row r="299" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
         <v>303</v>
       </c>
@@ -3935,92 +3947,48 @@
         <v>194</v>
       </c>
     </row>
-    <row r="300" spans="1:9">
+    <row r="300" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A300" s="6" t="s">
         <v>304</v>
       </c>
-      <c r="B300" s="19" t="s">
+      <c r="B300" s="18" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="301" spans="1:9">
+    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A301" s="7" t="s">
         <v>306</v>
       </c>
-      <c r="B301" s="20" t="s">
+      <c r="B301" s="19" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="303" spans="1:9">
-      <c r="E303" t="s">
-        <v>308</v>
-      </c>
-      <c r="I303">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="304" spans="1:9">
-      <c r="E304" t="s">
-        <v>309</v>
-      </c>
-      <c r="I304">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="305" spans="5:9">
-      <c r="E305" t="s">
-        <v>310</v>
-      </c>
-      <c r="I305">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="306" spans="5:9">
-      <c r="E306" t="s">
-        <v>311</v>
-      </c>
-      <c r="I306">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="307" spans="5:9">
-      <c r="E307" t="s">
-        <v>312</v>
-      </c>
-      <c r="I307">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="308" spans="5:9">
-      <c r="E308" t="s">
-        <v>313</v>
-      </c>
+    <row r="310" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O310" s="10"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A301" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A301">
-      <sortCondition sortBy="cellColor" ref="A1:A301" dxfId="0"/>
-    </sortState>
-  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="bd61af73-7999-4cce-802c-efc978926a1d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="bd61af73-7999-4cce-802c-efc978926a1d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4207,13 +4175,38 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3299C097-C3CA-435B-981B-D4CF9CFCB14C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0764A12-6148-4F70-8E4E-9C6221173BB4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bd61af73-7999-4cce-802c-efc978926a1d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0764A12-6148-4F70-8E4E-9C6221173BB4}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3299C097-C3CA-435B-981B-D4CF9CFCB14C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76BCA711-5A5E-4BA0-A2E7-AB021BAC5153}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76BCA711-5A5E-4BA0-A2E7-AB021BAC5153}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="bd61af73-7999-4cce-802c-efc978926a1d"/>
+    <ds:schemaRef ds:uri="ee918b65-cae3-47bc-8c3b-c1f3bd6f0a29"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>